<commit_message>
28, 29 sep added info
</commit_message>
<xml_diff>
--- a/ExcelLab-Covid.xlsx
+++ b/ExcelLab-Covid.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arianna/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arianna/Desktop/ExcelLab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C676364-8D8F-8446-81E6-C34FBCCFE4A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BCF952-F3F2-9943-B14D-2B710FB47676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37420" yWindow="460" windowWidth="24140" windowHeight="17040" xr2:uid="{2DB62F66-4D63-0744-B465-17CF4A6A55CD}"/>
   </bookViews>
@@ -473,7 +473,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -579,10 +579,34 @@
       <c r="C11" s="3">
         <v>44102</v>
       </c>
+      <c r="D11">
+        <v>1454</v>
+      </c>
+      <c r="E11" s="4">
+        <v>722</v>
+      </c>
+      <c r="F11">
+        <v>2176</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C12" s="3">
         <v>44103</v>
+      </c>
+      <c r="D12">
+        <v>2176</v>
+      </c>
+      <c r="E12" s="5">
+        <v>-516</v>
+      </c>
+      <c r="F12">
+        <v>1660</v>
+      </c>
+      <c r="G12">
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added a chart w/data
</commit_message>
<xml_diff>
--- a/ExcelLab-Covid.xlsx
+++ b/ExcelLab-Covid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arianna/Desktop/ExcelLab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BCF952-F3F2-9943-B14D-2B710FB47676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC119B9-976F-9749-9E25-18C8F097C987}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37420" yWindow="460" windowWidth="24140" windowHeight="17040" xr2:uid="{2DB62F66-4D63-0744-B465-17CF4A6A55CD}"/>
   </bookViews>
@@ -173,6 +173,1284 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#Previous cases</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$8:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>44099</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44102</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44103</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44104</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44106</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44107</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$8:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1341</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1362</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1215</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1454</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2176</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-968E-944A-AF1F-7A20FEA5D9DD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#Increase or decrease of cases</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$8:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>44099</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44102</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44103</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44104</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44106</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44107</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$8:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-147</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>722</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-516</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-968E-944A-AF1F-7A20FEA5D9DD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$8:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>44099</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44102</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44103</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44104</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44106</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44107</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$8:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1362</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1215</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1454</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2176</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1660</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-968E-944A-AF1F-7A20FEA5D9DD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#Deaths</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$8:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>44099</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44102</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44103</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44104</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44106</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44107</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$8:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-968E-944A-AF1F-7A20FEA5D9DD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1434788303"/>
+        <c:axId val="1434784079"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1434788303"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1434784079"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1434784079"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1434788303"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2533650</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B6784D4-B2E2-334B-B807-3D471C0757DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -470,10 +1748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F7E316-CA0C-5A4F-9C36-F3F5E9E0CEE8}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -624,7 +1902,13 @@
         <v>44106</v>
       </c>
     </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C16" s="3">
+        <v>44107</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated the 30th previous #
</commit_message>
<xml_diff>
--- a/ExcelLab-Covid.xlsx
+++ b/ExcelLab-Covid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arianna/Desktop/ExcelLab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC119B9-976F-9749-9E25-18C8F097C987}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3608B6FF-6829-2E40-B63F-C4026B90D061}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37420" yWindow="460" windowWidth="24140" windowHeight="17040" xr2:uid="{2DB62F66-4D63-0744-B465-17CF4A6A55CD}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" xr2:uid="{2DB62F66-4D63-0744-B465-17CF4A6A55CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -317,6 +317,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2176</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1660</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1751,7 +1754,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1891,6 +1894,9 @@
       <c r="C13" s="3">
         <v>44104</v>
       </c>
+      <c r="D13">
+        <v>1660</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C14" s="3">

</xml_diff>

<commit_message>
sep 30th new update
</commit_message>
<xml_diff>
--- a/ExcelLab-Covid.xlsx
+++ b/ExcelLab-Covid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arianna/Desktop/ExcelLab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3608B6FF-6829-2E40-B63F-C4026B90D061}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253A0632-EE71-2842-A6E3-DCA01553E3D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" xr2:uid="{2DB62F66-4D63-0744-B465-17CF4A6A55CD}"/>
+    <workbookView xWindow="-29760" yWindow="460" windowWidth="28800" windowHeight="16560" xr2:uid="{2DB62F66-4D63-0744-B465-17CF4A6A55CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -426,6 +426,9 @@
                 <c:pt idx="4">
                   <c:v>-516</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>137</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -531,6 +534,9 @@
                 <c:pt idx="4">
                   <c:v>1660</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>1797</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -635,6 +641,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1754,7 +1763,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1897,6 +1906,15 @@
       <c r="D13">
         <v>1660</v>
       </c>
+      <c r="E13" s="4">
+        <v>137</v>
+      </c>
+      <c r="F13">
+        <v>1797</v>
+      </c>
+      <c r="G13">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C14" s="3">

</xml_diff>